<commit_message>
add: new endpoints to handle emails and responses
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -5,13 +5,17 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Cuestionario General" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Cuestionario social_AA" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Cuestionario social_DA" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="Cuestionario entrevista_AA" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="Cuestionario entrevista_DA" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="79">
   <si>
     <t>ID registro</t>
   </si>
@@ -80,6 +84,174 @@
   </si>
   <si>
     <t>Nunca</t>
+  </si>
+  <si>
+    <t>Al acercarte a una conversación grupal, ¿piensas que los demás no querrán hablar contigo?</t>
+  </si>
+  <si>
+    <t>Cuando hablo con alguien del otro sexo, ¿me preocupa constantemente que me juzgue?</t>
+  </si>
+  <si>
+    <t>Mientras estoy hablando, ¿me preocupa si lo que estoy diciendo es irrelevante o aburrido?</t>
+  </si>
+  <si>
+    <t>Después de hablar con alguien, ¿tiendo a sobrepensar y preocuparme por las cosas que dije durante la conversación?</t>
+  </si>
+  <si>
+    <t>Antes de acercarme a hablar con alguien que no conozco, ¿pienso que me va a rechazar o ignorar?</t>
+  </si>
+  <si>
+    <t>¿Siento que mi corazón late más rápido cuando estoy cerca de grupos de personas hablando?</t>
+  </si>
+  <si>
+    <t>Al acercarme a personas desconocidas, ¿siento que me empiezan a sudar las manos?</t>
+  </si>
+  <si>
+    <t>Cuando intento iniciar una conversación con alguien del otro sexo, ¿siento que mis manos o cuerpo tiemblan?</t>
+  </si>
+  <si>
+    <t>¿Siento que mi cuerpo se tensa cuando estoy rodeado de personas hablando?</t>
+  </si>
+  <si>
+    <t>¿Tiendo a evitar acercarme a grupos de personas para no tener que iniciar una conversación?</t>
+  </si>
+  <si>
+    <t>¿Prefiero quedarme en un rincón o un lugar aislado?</t>
+  </si>
+  <si>
+    <t>¿Tiendo a cruzar los brazos o evitar el contacto visual para sentirme más cómodo/a?</t>
+  </si>
+  <si>
+    <t>Si me siento incómodo/a, ¿suelo buscar una excusa para irme lo más rápido posible?</t>
+  </si>
+  <si>
+    <t>Cuando hablo con gente nueva, ¿a menudo me encuentro tartamudeando o teniendo dificultad para encontrar las palabras correctas?</t>
+  </si>
+  <si>
+    <t>Al acercarte a una conversación grupal después de usar la aplicación, ¿sientes que ahora te resulta más fácil pensar que los demás querrán hablar contigo?</t>
+  </si>
+  <si>
+    <t>Después de usar la aplicación, ¿sientes que te preocupa menos que alguien del otro sexo te juzgue mientras hablas?</t>
+  </si>
+  <si>
+    <t>Después de usar la aplicación, ¿te preocupa menos si lo que estás diciendo es irrelevante o aburrido?</t>
+  </si>
+  <si>
+    <t>Tras utilizar la aplicación, ¿sientes que ya no sobrepiensas tanto ni te preocupas tanto por las cosas que dijiste en una conversación?</t>
+  </si>
+  <si>
+    <t>Después de usar la aplicación, ¿crees que piensas menos que serás rechazado/a o ignorado/a antes de acercarte a alguien que no conoces?</t>
+  </si>
+  <si>
+    <t>¿Sientes que, después de usar la aplicación, tu corazón late menos rápido cuando te acercas a grupos de personas hablando?</t>
+  </si>
+  <si>
+    <t>Tras el uso de la aplicación, ¿sientes que te sudan menos las manos al acercarte a personas desconocidas?</t>
+  </si>
+  <si>
+    <t>Después de usar la aplicación, ¿sientes menos temblores en tus manos o cuerpo cuando intentas iniciar una conversación con alguien del otro sexo?</t>
+  </si>
+  <si>
+    <t>¿Te sientes menos tenso/a cuando estás rodeado/a de personas hablando, después de haber usado la aplicación?</t>
+  </si>
+  <si>
+    <t>Después de usar la aplicación, ¿sientes que evitas menos acercarte a grupos de personas para iniciar una conversación?</t>
+  </si>
+  <si>
+    <t>¿Te sientes más cómodo/a al estar en el centro de la acción, en lugar de preferir un rincón o lugar aislado, después de usar la aplicación?</t>
+  </si>
+  <si>
+    <t>Después de usar la aplicación, ¿tiendes a cruzar menos los brazos o a evitar el contacto visual para sentirte más cómodo/a?</t>
+  </si>
+  <si>
+    <t>¿Sientes que, tras usar la aplicación, buscas menos excusas para irte rápidamente cuando te sientes incómodo/a?</t>
+  </si>
+  <si>
+    <t>Después de haber usado la aplicación, ¿sientes que tartamudeas menos o tienes menos dificultad para encontrar las palabras correctas al hablar con gente nueva?</t>
+  </si>
+  <si>
+    <t>Antes de responder una pregunta en una entrevista, ¿te preocupa decir algo incorrecto?</t>
+  </si>
+  <si>
+    <t>Durante la entrevista, ¿te preocupa constantemente que el entrevistador te esté juzgando negativamente?</t>
+  </si>
+  <si>
+    <t>Durante la entrevista, ¿piensas que no eres lo suficientemente bueno para la posición?</t>
+  </si>
+  <si>
+    <t>Antes de una entrevista laboral, ¿a menudo piensas en cancelar o evitar la entrevista por miedo o sentirte muy ansioso?</t>
+  </si>
+  <si>
+    <t>Después de una entrevista, ¿tiendes a repasar mentalmente todas las respuestas que diste y a criticarte por los errores?</t>
+  </si>
+  <si>
+    <t>Durante una entrevista laboral, ¿sientes que tu corazón late con mayor intensidad?</t>
+  </si>
+  <si>
+    <t>¿Sientes que tus manos o frente comienzan a sudar cuando estás en una entrevista laboral?</t>
+  </si>
+  <si>
+    <t>Durante una entrevista, ¿notas que tu voz suena tensa o temblorosa cuando hablas?</t>
+  </si>
+  <si>
+    <t>¿Sientes que tus músculos se tensan cuando estás siendo entrevistado/a?</t>
+  </si>
+  <si>
+    <t>Mientras estás siendo entrevistado/a, ¿tiendes a cruzar los brazos o adoptar una postura cerrada para sentirme más seguro/a?</t>
+  </si>
+  <si>
+    <t>Durante una entrevista, ¿te cuesta mantener el contacto visual con el entrevistador?</t>
+  </si>
+  <si>
+    <t>Durante la entrevista, ¿tiendes a jugar tus manos, morderte los labios o hacer movimientos repetitivos para lidiar con la ansiedad?</t>
+  </si>
+  <si>
+    <t>¿Qué tan a menudo recurres a comportamientos de evitación, como revisar el celular o mirar hacia otro lado, cuando estás en la entrevista laboral?</t>
+  </si>
+  <si>
+    <t>Cuando te hacen una pregunta difícil, ¿intentas cambiar de tema o desviar la conversación durante la entrevista?</t>
+  </si>
+  <si>
+    <t>Después de usar la aplicación, ¿te preocupa menos decir algo incorrecto antes de responder una pregunta en una entrevista?</t>
+  </si>
+  <si>
+    <t>Sientes que, tras usar la aplicación, ¿te preocupa menos que el entrevistador te esté juzgando negativamente durante la entrevista?</t>
+  </si>
+  <si>
+    <t>Después de usar la aplicación, ¿te sientes más seguro/a y piensas menos que no eres lo suficientemente bueno/a para la posición?</t>
+  </si>
+  <si>
+    <t>Tras utilizar la aplicación, ¿piensas menos en cancelar o evitar la entrevista por miedo o ansiedad?</t>
+  </si>
+  <si>
+    <t>Después de usar la aplicación, ¿tiendes a repasar menos mentalmente las respuestas que diste y a criticarte menos por posibles errores?</t>
+  </si>
+  <si>
+    <t>¿Sientes que tu corazón late con menos intensidad durante una entrevista laboral después de usar la aplicación?</t>
+  </si>
+  <si>
+    <t>¿Notas que tus manos o frente sudan menos durante una entrevista laboral después de usar la aplicación?</t>
+  </si>
+  <si>
+    <t>Después de usar la aplicación, ¿sientes que tu voz suena menos tensa o temblorosa cuando hablas durante una entrevista?</t>
+  </si>
+  <si>
+    <t>¿Sientes que tus músculos se tensan menos cuando estás siendo entrevistado/a tras usar la aplicación?</t>
+  </si>
+  <si>
+    <t>Después de usar la aplicación, ¿tiendes a cruzar menos los brazos o adoptar una postura cerrada durante una entrevista laboral?</t>
+  </si>
+  <si>
+    <t>¿Te resulta más fácil mantener el contacto visual con el entrevistador después de haber usado la aplicación?</t>
+  </si>
+  <si>
+    <t>¿Notas que juegas menos con tus manos, te muerdes menos los labios o haces menos movimientos repetitivos durante la entrevista después de usar la aplicación?</t>
+  </si>
+  <si>
+    <t>Tras el uso de la aplicación, ¿recurres menos a comportamientos de evitación, como revisar el celular o mirar hacia otro lado, durante la entrevista laboral?</t>
+  </si>
+  <si>
+    <t>¿Sientes que, después de usar la aplicación, intentas menos desviar la conversación o cambiar de tema cuando te hacen una pregunta difícil en una entrevista?</t>
   </si>
 </sst>
 </file>
@@ -742,4 +914,664 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>99016459</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45544</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>95830489</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45544</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>55346136</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45544</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>61013099</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45544</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>36472976</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45544</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10062696</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45544</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>98562949</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45544</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>99511656</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45544</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>